<commit_message>
scylla output done - checking for simulation conformance
</commit_message>
<xml_diff>
--- a/inputs/CostsxResources.xlsx
+++ b/inputs/CostsxResources.xlsx
@@ -447,7 +447,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D27"/>
+      <selection activeCell="C1" sqref="C1:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,11 +465,11 @@
       </c>
       <c r="C1">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D1" t="str">
         <f ca="1">CONCATENATE("&lt;resource ","key=",CHAR(34),B1,CHAR(34)," ", "value=",CHAR(34),C1,CHAR(34),"/&gt;")</f>
-        <v>&lt;resource key="Penn Osterwalder" value="10"/&gt;</v>
+        <v>&lt;resource key="Penn Osterwalder" value="27"/&gt;</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -481,11 +481,11 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C27" ca="1" si="0">RANDBETWEEN(1,30)</f>
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D27" ca="1" si="1">CONCATENATE("&lt;resource ","key=",CHAR(34),B2,CHAR(34)," ", "value=",CHAR(34),C2,CHAR(34),"/&gt;")</f>
-        <v>&lt;resource key="Nico Ojenbeer" value="18"/&gt;</v>
+        <v>&lt;resource key="Nico Ojenbeer" value="30"/&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -497,11 +497,11 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Elvira Lores" value="11"/&gt;</v>
+        <v>&lt;resource key="Elvira Lores" value="8"/&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -513,11 +513,11 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Miu Hanwan" value="7"/&gt;</v>
+        <v>&lt;resource key="Miu Hanwan" value="22"/&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -529,11 +529,11 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Fjodor Kowalski" value="24"/&gt;</v>
+        <v>&lt;resource key="Fjodor Kowalski" value="23"/&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -545,11 +545,11 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Immanuel Karagianni" value="16"/&gt;</v>
+        <v>&lt;resource key="Immanuel Karagianni" value="13"/&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -561,11 +561,11 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Clement Duchot" value="2"/&gt;</v>
+        <v>&lt;resource key="Clement Duchot" value="28"/&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -577,11 +577,11 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Kim Passa" value="21"/&gt;</v>
+        <v>&lt;resource key="Kim Passa" value="13"/&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -593,11 +593,11 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Christian Francois" value="24"/&gt;</v>
+        <v>&lt;resource key="Christian Francois" value="12"/&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -609,11 +609,11 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Alberto Duport" value="22"/&gt;</v>
+        <v>&lt;resource key="Alberto Duport" value="9"/&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -625,11 +625,11 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Esmana Liubiata" value="18"/&gt;</v>
+        <v>&lt;resource key="Esmana Liubiata" value="20"/&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -641,11 +641,11 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Tesca Lobes" value="28"/&gt;</v>
+        <v>&lt;resource key="Tesca Lobes" value="4"/&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -657,11 +657,11 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Anne Olwada" value="26"/&gt;</v>
+        <v>&lt;resource key="Anne Olwada" value="27"/&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -673,11 +673,11 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Anna Kaufmann" value="29"/&gt;</v>
+        <v>&lt;resource key="Anna Kaufmann" value="27"/&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -689,11 +689,11 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Sean Manney" value="24"/&gt;</v>
+        <v>&lt;resource key="Sean Manney" value="25"/&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -705,11 +705,11 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Carmen Finacse" value="17"/&gt;</v>
+        <v>&lt;resource key="Carmen Finacse" value="14"/&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -721,11 +721,11 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Kiu Kan" value="4"/&gt;</v>
+        <v>&lt;resource key="Kiu Kan" value="14"/&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -737,11 +737,11 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Esmeralda Clay" value="11"/&gt;</v>
+        <v>&lt;resource key="Esmeralda Clay" value="12"/&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -753,11 +753,11 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Karen Clarens" value="9"/&gt;</v>
+        <v>&lt;resource key="Karen Clarens" value="7"/&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -785,11 +785,11 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Maris Freeman" value="7"/&gt;</v>
+        <v>&lt;resource key="Maris Freeman" value="2"/&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -801,11 +801,11 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Heinz Gutschmidt" value="18"/&gt;</v>
+        <v>&lt;resource key="Heinz Gutschmidt" value="15"/&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -817,11 +817,11 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Magdalena Predutta" value="14"/&gt;</v>
+        <v>&lt;resource key="Magdalena Predutta" value="10"/&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -833,11 +833,11 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Francois de Perrier" value="29"/&gt;</v>
+        <v>&lt;resource key="Francois de Perrier" value="11"/&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -849,11 +849,11 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Karel de Groot" value="24"/&gt;</v>
+        <v>&lt;resource key="Karel de Groot" value="6"/&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -865,11 +865,11 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Pedro Alvares" value="30"/&gt;</v>
+        <v>&lt;resource key="Pedro Alvares" value="28"/&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -881,11 +881,11 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>&lt;resource key="Karalda Nimwada" value="11"/&gt;</v>
+        <v>&lt;resource key="Karalda Nimwada" value="4"/&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>